<commit_message>
Paquete y Actualizacion Configuracion De Proyecto
</commit_message>
<xml_diff>
--- a/Traduccion.xlsx
+++ b/Traduccion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desarrollo\CSharp\Aprender\Sistema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A6F4832-F054-4F04-A499-7F5D4744E0FC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489225FF-C6D4-464A-A93D-46A47B22B4F2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="3975" xr2:uid="{DF80EA25-F23F-4F58-BCA7-1CB9AD1F7B23}"/>
   </bookViews>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>checkout</t>
   </si>
   <si>
-    <t>Revisa</t>
-  </si>
-  <si>
     <t>feature</t>
   </si>
   <si>
@@ -55,13 +52,51 @@
   </si>
   <si>
     <t>Rama</t>
+  </si>
+  <si>
+    <t>fetch </t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>dominar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git-pull </t>
+  </si>
+  <si>
+    <t>Obtenga e integre con otro repositorio o una sucursal local</t>
+  </si>
+  <si>
+    <r>
+      <t>Es importante tener en cuenta que el comando </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFF14E32"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>fetch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF4E443C"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t> sólo recupera la información y la pone en tu repositorio local —no la une automáticamente con tu trabajo ni modifica aquello en lo que estás trabajando.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,10 +105,28 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="23"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF4E443C"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFF14E32"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -96,9 +149,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,48 +468,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BDF9E75-3F73-4150-ADD9-EF422CC3058F}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="87.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>